<commit_message>
Revert "Merge branch 'master' of https://github.com/satotodob/D_Group_project"
This reverts commit 34322ccd064d3a38f722eaaf5678bc8e8be49a10, reversing
changes made to 54817881ecb4c61e9e47c34e22b3caa91c3939c4.
</commit_message>
<xml_diff>
--- a/テスト仕様書/テスト仕様書_STEP1.xlsx
+++ b/テスト仕様書/テスト仕様書_STEP1.xlsx
@@ -47,7 +47,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="340" uniqueCount="182">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="333" uniqueCount="173">
   <si>
     <t>NO</t>
     <phoneticPr fontId="1"/>
@@ -1668,6 +1668,10 @@
     <phoneticPr fontId="1"/>
   </si>
   <si>
+    <t>存在するIDに適当な1文字を追加し、存在しないIDに変えてログインを試す</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
     <t>パスワード誤入力</t>
     <rPh sb="5" eb="8">
       <t>ゴニュウリョク</t>
@@ -1693,6 +1697,25 @@
     </rPh>
     <rPh sb="31" eb="33">
       <t>ヒョウジ</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>存在するIDに対するパスワード末尾1文字を消してfalse判定にする</t>
+    <rPh sb="7" eb="8">
+      <t>タイ</t>
+    </rPh>
+    <rPh sb="15" eb="17">
+      <t>マツビ</t>
+    </rPh>
+    <rPh sb="18" eb="20">
+      <t>モジ</t>
+    </rPh>
+    <rPh sb="21" eb="22">
+      <t>ケ</t>
+    </rPh>
+    <rPh sb="29" eb="31">
+      <t>ハンテイ</t>
     </rPh>
     <phoneticPr fontId="1"/>
   </si>
@@ -2399,109 +2422,6 @@
     </rPh>
     <phoneticPr fontId="1"/>
   </si>
-  <si>
-    <t>存在するIDに適当な1文字を追加し、存在しないIDに変えてログインを試す
-ID：店長あ　で試す（正式なID店長）</t>
-    <rPh sb="40" eb="42">
-      <t>テンチョウ</t>
-    </rPh>
-    <rPh sb="45" eb="46">
-      <t>タメ</t>
-    </rPh>
-    <rPh sb="48" eb="50">
-      <t>セイシキ</t>
-    </rPh>
-    <rPh sb="53" eb="55">
-      <t>テンチョウ</t>
-    </rPh>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>存在するIDに対するパスワード末尾1文字を消してfalse判定にする
-パスワード：test123 で試す（正式なパスワード　test1234）</t>
-    <rPh sb="7" eb="8">
-      <t>タイ</t>
-    </rPh>
-    <rPh sb="15" eb="17">
-      <t>マツビ</t>
-    </rPh>
-    <rPh sb="18" eb="20">
-      <t>モジ</t>
-    </rPh>
-    <rPh sb="21" eb="22">
-      <t>ケ</t>
-    </rPh>
-    <rPh sb="29" eb="31">
-      <t>ハンテイ</t>
-    </rPh>
-    <rPh sb="50" eb="51">
-      <t>タメ</t>
-    </rPh>
-    <rPh sb="53" eb="55">
-      <t>セイシキ</t>
-    </rPh>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>ID：店長　パスワード：test1234</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>ログインユーザー名：店長</t>
-    <rPh sb="8" eb="9">
-      <t>メイ</t>
-    </rPh>
-    <rPh sb="10" eb="12">
-      <t>テンチョウ</t>
-    </rPh>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>ユーザー名：店長</t>
-    <rPh sb="4" eb="5">
-      <t>メイ</t>
-    </rPh>
-    <rPh sb="6" eb="8">
-      <t>テンチョウ</t>
-    </rPh>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>選択メニュー「きたあかりバター」</t>
-    <rPh sb="0" eb="2">
-      <t>センタク</t>
-    </rPh>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>選択メニュー「きたあかりバター」の数量1　確定押下後</t>
-    <rPh sb="17" eb="19">
-      <t>スウリョウ</t>
-    </rPh>
-    <rPh sb="21" eb="23">
-      <t>カクテイ</t>
-    </rPh>
-    <rPh sb="23" eb="26">
-      <t>オウカゴ</t>
-    </rPh>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>選択メニュー「オレンジジュース」</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>選択メニュー「オレンジジュース」の数量1　確定押下後</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>選択メニュー「おにぎり」</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>選択メニュー「おにぎり」の数量1　確定押下後</t>
-    <phoneticPr fontId="1"/>
-  </si>
 </sst>
 </file>
 
@@ -2534,14 +2454,15 @@
     </font>
     <font>
       <sz val="11"/>
-      <color theme="1"/>
+      <color rgb="FFFF0000"/>
       <name val="ＭＳ Ｐゴシック"/>
-      <family val="3"/>
+      <family val="2"/>
       <charset val="128"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
+      <color theme="1"/>
       <name val="ＭＳ Ｐゴシック"/>
       <family val="3"/>
       <charset val="128"/>
@@ -2716,10 +2637,10 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1">
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
   </cellXfs>
@@ -3005,7 +2926,7 @@
   <dimension ref="A1:L43"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D14" sqref="D14"/>
+      <selection activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
@@ -3077,7 +2998,7 @@
         <v>37</v>
       </c>
       <c r="D5" s="4" t="s">
-        <v>165</v>
+        <v>167</v>
       </c>
       <c r="E5" s="2"/>
       <c r="F5" s="2"/>
@@ -3164,7 +3085,7 @@
       <c r="K9" s="1"/>
       <c r="L9" s="1"/>
     </row>
-    <row r="10" spans="1:12" ht="40.5" x14ac:dyDescent="0.15">
+    <row r="10" spans="1:12" ht="27" x14ac:dyDescent="0.15">
       <c r="A10" s="9">
         <v>7</v>
       </c>
@@ -3175,7 +3096,7 @@
         <v>125</v>
       </c>
       <c r="D10" s="20" t="s">
-        <v>171</v>
+        <v>126</v>
       </c>
       <c r="E10" s="2"/>
       <c r="F10" s="2"/>
@@ -3186,18 +3107,18 @@
       <c r="K10" s="1"/>
       <c r="L10" s="1"/>
     </row>
-    <row r="11" spans="1:12" ht="54" x14ac:dyDescent="0.15">
+    <row r="11" spans="1:12" ht="27" x14ac:dyDescent="0.15">
       <c r="A11" s="9">
         <v>8</v>
       </c>
       <c r="B11" s="4" t="s">
-        <v>126</v>
+        <v>127</v>
       </c>
       <c r="C11" s="4" t="s">
-        <v>127</v>
+        <v>128</v>
       </c>
       <c r="D11" s="19" t="s">
-        <v>172</v>
+        <v>129</v>
       </c>
       <c r="E11" s="2"/>
       <c r="F11" s="2"/>
@@ -3213,13 +3134,13 @@
         <v>9</v>
       </c>
       <c r="B12" s="4" t="s">
-        <v>128</v>
+        <v>130</v>
       </c>
       <c r="C12" s="4" t="s">
-        <v>129</v>
+        <v>131</v>
       </c>
       <c r="D12" s="2" t="s">
-        <v>130</v>
+        <v>132</v>
       </c>
       <c r="E12" s="2"/>
       <c r="F12" s="2"/>
@@ -3235,14 +3156,12 @@
         <v>10</v>
       </c>
       <c r="B13" s="4" t="s">
-        <v>128</v>
+        <v>130</v>
       </c>
       <c r="C13" s="4" t="s">
-        <v>131</v>
-      </c>
-      <c r="D13" s="19" t="s">
-        <v>173</v>
-      </c>
+        <v>133</v>
+      </c>
+      <c r="D13" s="19"/>
       <c r="E13" s="2"/>
       <c r="F13" s="2"/>
       <c r="G13" s="10"/>
@@ -4858,646 +4777,6 @@
   <dimension ref="A1:L43"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D9" sqref="D9"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
-  <cols>
-    <col min="1" max="1" width="3.25" customWidth="1"/>
-    <col min="2" max="2" width="17.375" customWidth="1"/>
-    <col min="3" max="3" width="57.625" customWidth="1"/>
-    <col min="4" max="4" width="45.125" customWidth="1"/>
-    <col min="5" max="5" width="12.625" customWidth="1"/>
-    <col min="6" max="6" width="11.625" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:12" ht="17.25" x14ac:dyDescent="0.15">
-      <c r="A1" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="C1" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.15">
-      <c r="A3" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="B3" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="C3" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="D3" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="E3" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="F3" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="G3" s="5" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="4" spans="1:12" ht="27" x14ac:dyDescent="0.15">
-      <c r="A4" s="9">
-        <v>1</v>
-      </c>
-      <c r="B4" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="C4" s="4" t="s">
-        <v>40</v>
-      </c>
-      <c r="D4" s="4" t="s">
-        <v>132</v>
-      </c>
-      <c r="E4" s="2"/>
-      <c r="F4" s="2"/>
-      <c r="G4" s="10"/>
-    </row>
-    <row r="5" spans="1:12" ht="27" x14ac:dyDescent="0.15">
-      <c r="A5" s="9">
-        <v>2</v>
-      </c>
-      <c r="B5" s="4" t="s">
-        <v>9</v>
-      </c>
-      <c r="C5" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="D5" s="17" t="s">
-        <v>164</v>
-      </c>
-      <c r="E5" s="2"/>
-      <c r="F5" s="2"/>
-      <c r="G5" s="10"/>
-    </row>
-    <row r="6" spans="1:12" ht="27" x14ac:dyDescent="0.15">
-      <c r="A6" s="9">
-        <v>3</v>
-      </c>
-      <c r="B6" s="8" t="s">
-        <v>41</v>
-      </c>
-      <c r="C6" s="8" t="s">
-        <v>42</v>
-      </c>
-      <c r="D6" s="22" t="s">
-        <v>174</v>
-      </c>
-      <c r="E6" s="2"/>
-      <c r="F6" s="2"/>
-      <c r="G6" s="10"/>
-    </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.15">
-      <c r="A7" s="9">
-        <v>4</v>
-      </c>
-      <c r="B7" s="4" t="s">
-        <v>133</v>
-      </c>
-      <c r="C7" s="2" t="s">
-        <v>134</v>
-      </c>
-      <c r="D7" s="2"/>
-      <c r="E7" s="2"/>
-      <c r="F7" s="2"/>
-      <c r="G7" s="10"/>
-      <c r="H7" s="1"/>
-      <c r="I7" s="1"/>
-      <c r="J7" s="1"/>
-      <c r="K7" s="1"/>
-      <c r="L7" s="1"/>
-    </row>
-    <row r="8" spans="1:12" ht="27" x14ac:dyDescent="0.15">
-      <c r="A8" s="9">
-        <v>5</v>
-      </c>
-      <c r="B8" s="4" t="s">
-        <v>135</v>
-      </c>
-      <c r="C8" s="4" t="s">
-        <v>136</v>
-      </c>
-      <c r="D8" s="2" t="s">
-        <v>137</v>
-      </c>
-      <c r="E8" s="2"/>
-      <c r="F8" s="2"/>
-      <c r="G8" s="10"/>
-      <c r="H8" s="1"/>
-      <c r="I8" s="1"/>
-      <c r="J8" s="1"/>
-      <c r="K8" s="1"/>
-      <c r="L8" s="1"/>
-    </row>
-    <row r="9" spans="1:12" ht="27" x14ac:dyDescent="0.15">
-      <c r="A9" s="9">
-        <v>6</v>
-      </c>
-      <c r="B9" s="4" t="s">
-        <v>138</v>
-      </c>
-      <c r="C9" s="4" t="s">
-        <v>139</v>
-      </c>
-      <c r="D9" s="2" t="s">
-        <v>140</v>
-      </c>
-      <c r="E9" s="2"/>
-      <c r="F9" s="2"/>
-      <c r="G9" s="10"/>
-      <c r="H9" s="1"/>
-      <c r="I9" s="1"/>
-      <c r="J9" s="1"/>
-      <c r="K9" s="1"/>
-      <c r="L9" s="1"/>
-    </row>
-    <row r="10" spans="1:12" ht="27" x14ac:dyDescent="0.15">
-      <c r="A10" s="9">
-        <v>7</v>
-      </c>
-      <c r="B10" s="4" t="s">
-        <v>141</v>
-      </c>
-      <c r="C10" s="4" t="s">
-        <v>142</v>
-      </c>
-      <c r="D10" s="2" t="s">
-        <v>38</v>
-      </c>
-      <c r="E10" s="2"/>
-      <c r="F10" s="2"/>
-      <c r="G10" s="10"/>
-      <c r="H10" s="1"/>
-      <c r="I10" s="1"/>
-      <c r="J10" s="1"/>
-      <c r="K10" s="1"/>
-      <c r="L10" s="1"/>
-    </row>
-    <row r="11" spans="1:12" x14ac:dyDescent="0.15">
-      <c r="A11" s="9">
-        <v>8</v>
-      </c>
-      <c r="B11" s="4" t="s">
-        <v>43</v>
-      </c>
-      <c r="C11" s="4" t="s">
-        <v>143</v>
-      </c>
-      <c r="D11" s="4"/>
-      <c r="E11" s="2"/>
-      <c r="F11" s="2"/>
-      <c r="G11" s="10"/>
-      <c r="H11" s="1"/>
-      <c r="I11" s="1"/>
-      <c r="J11" s="1"/>
-      <c r="K11" s="1"/>
-      <c r="L11" s="1"/>
-    </row>
-    <row r="12" spans="1:12" x14ac:dyDescent="0.15">
-      <c r="A12" s="9">
-        <v>9</v>
-      </c>
-      <c r="B12" s="4"/>
-      <c r="C12" s="4"/>
-      <c r="D12" s="4"/>
-      <c r="E12" s="2"/>
-      <c r="F12" s="2"/>
-      <c r="G12" s="10"/>
-      <c r="H12" s="1"/>
-      <c r="I12" s="1"/>
-      <c r="J12" s="1"/>
-      <c r="K12" s="1"/>
-      <c r="L12" s="1"/>
-    </row>
-    <row r="13" spans="1:12" x14ac:dyDescent="0.15">
-      <c r="A13" s="9">
-        <v>10</v>
-      </c>
-      <c r="B13" s="4"/>
-      <c r="C13" s="2"/>
-      <c r="D13" s="2"/>
-      <c r="E13" s="2"/>
-      <c r="F13" s="2"/>
-      <c r="G13" s="10"/>
-      <c r="H13" s="1"/>
-      <c r="I13" s="1"/>
-      <c r="J13" s="1"/>
-      <c r="K13" s="1"/>
-      <c r="L13" s="1"/>
-    </row>
-    <row r="14" spans="1:12" x14ac:dyDescent="0.15">
-      <c r="A14" s="9">
-        <v>11</v>
-      </c>
-      <c r="B14" s="2"/>
-      <c r="C14" s="2"/>
-      <c r="D14" s="2"/>
-      <c r="E14" s="2"/>
-      <c r="F14" s="2"/>
-      <c r="G14" s="10"/>
-      <c r="H14" s="1"/>
-      <c r="I14" s="1"/>
-      <c r="J14" s="1"/>
-      <c r="K14" s="1"/>
-      <c r="L14" s="1"/>
-    </row>
-    <row r="15" spans="1:12" x14ac:dyDescent="0.15">
-      <c r="A15" s="9">
-        <v>12</v>
-      </c>
-      <c r="B15" s="4"/>
-      <c r="C15" s="4"/>
-      <c r="D15" s="4"/>
-      <c r="E15" s="2"/>
-      <c r="F15" s="2"/>
-      <c r="G15" s="10"/>
-      <c r="H15" s="1"/>
-      <c r="I15" s="1"/>
-      <c r="J15" s="1"/>
-      <c r="K15" s="1"/>
-      <c r="L15" s="1"/>
-    </row>
-    <row r="16" spans="1:12" x14ac:dyDescent="0.15">
-      <c r="A16" s="9">
-        <v>13</v>
-      </c>
-      <c r="B16" s="4"/>
-      <c r="C16" s="4"/>
-      <c r="D16" s="4"/>
-      <c r="E16" s="2"/>
-      <c r="F16" s="2"/>
-      <c r="G16" s="10"/>
-      <c r="H16" s="1"/>
-      <c r="I16" s="1"/>
-      <c r="J16" s="1"/>
-      <c r="K16" s="1"/>
-      <c r="L16" s="1"/>
-    </row>
-    <row r="17" spans="1:12" x14ac:dyDescent="0.15">
-      <c r="A17" s="9">
-        <v>14</v>
-      </c>
-      <c r="B17" s="4"/>
-      <c r="C17" s="4"/>
-      <c r="D17" s="4"/>
-      <c r="E17" s="2"/>
-      <c r="F17" s="2"/>
-      <c r="G17" s="10"/>
-      <c r="H17" s="1"/>
-      <c r="I17" s="1"/>
-      <c r="J17" s="1"/>
-      <c r="K17" s="1"/>
-      <c r="L17" s="1"/>
-    </row>
-    <row r="18" spans="1:12" x14ac:dyDescent="0.15">
-      <c r="A18" s="9">
-        <v>15</v>
-      </c>
-      <c r="B18" s="4"/>
-      <c r="C18" s="4"/>
-      <c r="D18" s="4"/>
-      <c r="E18" s="2"/>
-      <c r="F18" s="2"/>
-      <c r="G18" s="10"/>
-      <c r="H18" s="1"/>
-      <c r="I18" s="1"/>
-      <c r="J18" s="1"/>
-      <c r="K18" s="1"/>
-      <c r="L18" s="1"/>
-    </row>
-    <row r="19" spans="1:12" x14ac:dyDescent="0.15">
-      <c r="A19" s="9">
-        <v>16</v>
-      </c>
-      <c r="B19" s="6"/>
-      <c r="C19" s="6"/>
-      <c r="D19" s="6"/>
-      <c r="E19" s="2"/>
-      <c r="F19" s="2"/>
-      <c r="G19" s="10"/>
-      <c r="H19" s="1"/>
-      <c r="I19" s="1"/>
-      <c r="J19" s="1"/>
-      <c r="K19" s="1"/>
-      <c r="L19" s="1"/>
-    </row>
-    <row r="20" spans="1:12" x14ac:dyDescent="0.15">
-      <c r="A20" s="9">
-        <v>17</v>
-      </c>
-      <c r="B20" s="4"/>
-      <c r="C20" s="4"/>
-      <c r="D20" s="6"/>
-      <c r="E20" s="2"/>
-      <c r="F20" s="2"/>
-      <c r="G20" s="10"/>
-      <c r="H20" s="1"/>
-      <c r="I20" s="1"/>
-      <c r="J20" s="1"/>
-      <c r="K20" s="1"/>
-      <c r="L20" s="1"/>
-    </row>
-    <row r="21" spans="1:12" x14ac:dyDescent="0.15">
-      <c r="A21" s="9">
-        <v>18</v>
-      </c>
-      <c r="B21" s="4"/>
-      <c r="C21" s="4"/>
-      <c r="D21" s="6"/>
-      <c r="E21" s="2"/>
-      <c r="F21" s="2"/>
-      <c r="G21" s="10"/>
-      <c r="H21" s="1"/>
-      <c r="I21" s="1"/>
-      <c r="J21" s="1"/>
-      <c r="K21" s="1"/>
-      <c r="L21" s="1"/>
-    </row>
-    <row r="22" spans="1:12" x14ac:dyDescent="0.15">
-      <c r="A22" s="9">
-        <v>19</v>
-      </c>
-      <c r="B22" s="4"/>
-      <c r="C22" s="4"/>
-      <c r="D22" s="6"/>
-      <c r="E22" s="2"/>
-      <c r="F22" s="2"/>
-      <c r="G22" s="10"/>
-      <c r="H22" s="1"/>
-      <c r="I22" s="1"/>
-      <c r="J22" s="1"/>
-      <c r="K22" s="1"/>
-      <c r="L22" s="1"/>
-    </row>
-    <row r="23" spans="1:12" x14ac:dyDescent="0.15">
-      <c r="A23" s="11">
-        <v>20</v>
-      </c>
-      <c r="B23" s="6"/>
-      <c r="C23" s="6"/>
-      <c r="D23" s="6"/>
-      <c r="E23" s="7"/>
-      <c r="F23" s="7"/>
-      <c r="G23" s="12"/>
-      <c r="H23" s="1"/>
-      <c r="I23" s="1"/>
-      <c r="J23" s="1"/>
-      <c r="K23" s="1"/>
-      <c r="L23" s="1"/>
-    </row>
-    <row r="24" spans="1:12" s="1" customFormat="1" x14ac:dyDescent="0.15">
-      <c r="A24" s="2">
-        <v>21</v>
-      </c>
-      <c r="B24" s="4"/>
-      <c r="C24" s="4"/>
-      <c r="D24" s="4"/>
-      <c r="E24" s="2"/>
-      <c r="F24" s="2"/>
-      <c r="G24" s="10"/>
-    </row>
-    <row r="25" spans="1:12" x14ac:dyDescent="0.15">
-      <c r="A25" s="13">
-        <v>22</v>
-      </c>
-      <c r="B25" s="14"/>
-      <c r="C25" s="14"/>
-      <c r="D25" s="15"/>
-      <c r="E25" s="15"/>
-      <c r="F25" s="15"/>
-      <c r="G25" s="16"/>
-      <c r="H25" s="1"/>
-      <c r="I25" s="1"/>
-      <c r="J25" s="1"/>
-      <c r="K25" s="1"/>
-      <c r="L25" s="1"/>
-    </row>
-    <row r="26" spans="1:12" x14ac:dyDescent="0.15">
-      <c r="A26" s="9">
-        <v>23</v>
-      </c>
-      <c r="B26" s="8"/>
-      <c r="C26" s="8"/>
-      <c r="D26" s="4"/>
-      <c r="E26" s="2"/>
-      <c r="F26" s="2"/>
-      <c r="G26" s="10"/>
-      <c r="H26" s="1"/>
-      <c r="I26" s="1"/>
-      <c r="J26" s="1"/>
-      <c r="K26" s="1"/>
-      <c r="L26" s="1"/>
-    </row>
-    <row r="27" spans="1:12" x14ac:dyDescent="0.15">
-      <c r="A27" s="9">
-        <v>24</v>
-      </c>
-      <c r="B27" s="8"/>
-      <c r="C27" s="8"/>
-      <c r="D27" s="4"/>
-      <c r="E27" s="2"/>
-      <c r="F27" s="2"/>
-      <c r="G27" s="10"/>
-      <c r="H27" s="1"/>
-      <c r="I27" s="1"/>
-      <c r="J27" s="1"/>
-      <c r="K27" s="1"/>
-      <c r="L27" s="1"/>
-    </row>
-    <row r="28" spans="1:12" x14ac:dyDescent="0.15">
-      <c r="A28" s="9">
-        <v>25</v>
-      </c>
-      <c r="B28" s="4"/>
-      <c r="C28" s="8"/>
-      <c r="D28" s="4"/>
-      <c r="E28" s="2"/>
-      <c r="F28" s="2"/>
-      <c r="G28" s="10"/>
-    </row>
-    <row r="29" spans="1:12" x14ac:dyDescent="0.15">
-      <c r="A29" s="9">
-        <v>26</v>
-      </c>
-      <c r="B29" s="4"/>
-      <c r="C29" s="8"/>
-      <c r="D29" s="4"/>
-      <c r="E29" s="2"/>
-      <c r="F29" s="2"/>
-      <c r="G29" s="10"/>
-    </row>
-    <row r="30" spans="1:12" x14ac:dyDescent="0.15">
-      <c r="A30" s="9">
-        <v>27</v>
-      </c>
-      <c r="B30" s="4"/>
-      <c r="C30" s="8"/>
-      <c r="D30" s="4"/>
-      <c r="E30" s="2"/>
-      <c r="F30" s="2"/>
-      <c r="G30" s="10"/>
-    </row>
-    <row r="31" spans="1:12" x14ac:dyDescent="0.15">
-      <c r="A31" s="9">
-        <v>28</v>
-      </c>
-      <c r="B31" s="4"/>
-      <c r="C31" s="8"/>
-      <c r="D31" s="4"/>
-      <c r="E31" s="2"/>
-      <c r="F31" s="2"/>
-      <c r="G31" s="10"/>
-    </row>
-    <row r="32" spans="1:12" x14ac:dyDescent="0.15">
-      <c r="A32" s="9">
-        <v>29</v>
-      </c>
-      <c r="B32" s="4"/>
-      <c r="C32" s="8"/>
-      <c r="D32" s="4"/>
-      <c r="E32" s="2"/>
-      <c r="F32" s="2"/>
-      <c r="G32" s="10"/>
-    </row>
-    <row r="33" spans="1:7" x14ac:dyDescent="0.15">
-      <c r="A33" s="9">
-        <v>30</v>
-      </c>
-      <c r="B33" s="4"/>
-      <c r="C33" s="8"/>
-      <c r="D33" s="4"/>
-      <c r="E33" s="2"/>
-      <c r="F33" s="2"/>
-      <c r="G33" s="10"/>
-    </row>
-    <row r="34" spans="1:7" x14ac:dyDescent="0.15">
-      <c r="A34" s="9">
-        <v>31</v>
-      </c>
-      <c r="B34" s="4"/>
-      <c r="C34" s="8"/>
-      <c r="D34" s="4"/>
-      <c r="E34" s="2"/>
-      <c r="F34" s="2"/>
-      <c r="G34" s="10"/>
-    </row>
-    <row r="35" spans="1:7" x14ac:dyDescent="0.15">
-      <c r="A35" s="9">
-        <v>32</v>
-      </c>
-      <c r="B35" s="4"/>
-      <c r="C35" s="8"/>
-      <c r="D35" s="4"/>
-      <c r="E35" s="2"/>
-      <c r="F35" s="2"/>
-      <c r="G35" s="10"/>
-    </row>
-    <row r="36" spans="1:7" x14ac:dyDescent="0.15">
-      <c r="A36" s="9">
-        <v>33</v>
-      </c>
-      <c r="B36" s="4"/>
-      <c r="C36" s="8"/>
-      <c r="D36" s="4"/>
-      <c r="E36" s="2"/>
-      <c r="F36" s="2"/>
-      <c r="G36" s="10"/>
-    </row>
-    <row r="37" spans="1:7" x14ac:dyDescent="0.15">
-      <c r="A37" s="9">
-        <v>34</v>
-      </c>
-      <c r="B37" s="4"/>
-      <c r="C37" s="8"/>
-      <c r="D37" s="4"/>
-      <c r="E37" s="2"/>
-      <c r="F37" s="2"/>
-      <c r="G37" s="10"/>
-    </row>
-    <row r="38" spans="1:7" x14ac:dyDescent="0.15">
-      <c r="A38" s="9">
-        <v>35</v>
-      </c>
-      <c r="B38" s="4"/>
-      <c r="C38" s="8"/>
-      <c r="D38" s="4"/>
-      <c r="E38" s="2"/>
-      <c r="F38" s="2"/>
-      <c r="G38" s="10"/>
-    </row>
-    <row r="39" spans="1:7" x14ac:dyDescent="0.15">
-      <c r="A39" s="9">
-        <v>36</v>
-      </c>
-      <c r="B39" s="4"/>
-      <c r="C39" s="8"/>
-      <c r="D39" s="4"/>
-      <c r="E39" s="2"/>
-      <c r="F39" s="2"/>
-      <c r="G39" s="10"/>
-    </row>
-    <row r="40" spans="1:7" x14ac:dyDescent="0.15">
-      <c r="A40" s="9">
-        <v>37</v>
-      </c>
-      <c r="B40" s="4"/>
-      <c r="C40" s="8"/>
-      <c r="D40" s="4"/>
-      <c r="E40" s="2"/>
-      <c r="F40" s="2"/>
-      <c r="G40" s="10"/>
-    </row>
-    <row r="41" spans="1:7" x14ac:dyDescent="0.15">
-      <c r="A41" s="9">
-        <v>38</v>
-      </c>
-      <c r="B41" s="4"/>
-      <c r="C41" s="4"/>
-      <c r="D41" s="4"/>
-      <c r="E41" s="2"/>
-      <c r="F41" s="2"/>
-      <c r="G41" s="10"/>
-    </row>
-    <row r="42" spans="1:7" x14ac:dyDescent="0.15">
-      <c r="A42" s="9">
-        <v>39</v>
-      </c>
-      <c r="B42" s="4"/>
-      <c r="C42" s="4"/>
-      <c r="D42" s="4"/>
-      <c r="E42" s="2"/>
-      <c r="F42" s="2"/>
-      <c r="G42" s="10"/>
-    </row>
-    <row r="43" spans="1:7" x14ac:dyDescent="0.15">
-      <c r="A43" s="9">
-        <v>40</v>
-      </c>
-      <c r="B43" s="4"/>
-      <c r="C43" s="4"/>
-      <c r="D43" s="4"/>
-      <c r="E43" s="2"/>
-      <c r="F43" s="2"/>
-      <c r="G43" s="10"/>
-    </row>
-  </sheetData>
-  <phoneticPr fontId="1"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="360" verticalDpi="360" r:id="rId1"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:L43"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
       <selection activeCell="D5" sqref="D5"/>
     </sheetView>
   </sheetViews>
@@ -5516,7 +4795,7 @@
         <v>7</v>
       </c>
       <c r="C1" t="s">
-        <v>51</v>
+        <v>39</v>
       </c>
     </row>
     <row r="3" spans="1:12" x14ac:dyDescent="0.15">
@@ -5542,7 +4821,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.15">
+    <row r="4" spans="1:12" ht="27" x14ac:dyDescent="0.15">
       <c r="A4" s="9">
         <v>1</v>
       </c>
@@ -5550,10 +4829,10 @@
         <v>8</v>
       </c>
       <c r="C4" s="4" t="s">
-        <v>45</v>
-      </c>
-      <c r="D4" s="2" t="s">
-        <v>144</v>
+        <v>40</v>
+      </c>
+      <c r="D4" s="4" t="s">
+        <v>134</v>
       </c>
       <c r="E4" s="2"/>
       <c r="F4" s="2"/>
@@ -5564,48 +4843,44 @@
         <v>2</v>
       </c>
       <c r="B5" s="4" t="s">
-        <v>46</v>
+        <v>9</v>
       </c>
       <c r="C5" s="4" t="s">
-        <v>47</v>
-      </c>
-      <c r="D5" s="19" t="s">
-        <v>175</v>
+        <v>10</v>
+      </c>
+      <c r="D5" s="17" t="s">
+        <v>166</v>
       </c>
       <c r="E5" s="2"/>
       <c r="F5" s="2"/>
       <c r="G5" s="10"/>
     </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.15">
+    <row r="6" spans="1:12" ht="27" x14ac:dyDescent="0.15">
       <c r="A6" s="9">
         <v>3</v>
       </c>
-      <c r="B6" s="4" t="s">
-        <v>48</v>
-      </c>
-      <c r="C6" s="4" t="s">
-        <v>50</v>
-      </c>
-      <c r="D6" s="2" t="s">
-        <v>145</v>
-      </c>
+      <c r="B6" s="8" t="s">
+        <v>41</v>
+      </c>
+      <c r="C6" s="8" t="s">
+        <v>42</v>
+      </c>
+      <c r="D6" s="21"/>
       <c r="E6" s="2"/>
       <c r="F6" s="2"/>
       <c r="G6" s="10"/>
     </row>
-    <row r="7" spans="1:12" ht="27" x14ac:dyDescent="0.15">
+    <row r="7" spans="1:12" x14ac:dyDescent="0.15">
       <c r="A7" s="9">
         <v>4</v>
       </c>
-      <c r="B7" s="2" t="s">
-        <v>49</v>
-      </c>
-      <c r="C7" s="4" t="s">
-        <v>146</v>
-      </c>
-      <c r="D7" s="2" t="s">
-        <v>147</v>
-      </c>
+      <c r="B7" s="4" t="s">
+        <v>135</v>
+      </c>
+      <c r="C7" s="2" t="s">
+        <v>136</v>
+      </c>
+      <c r="D7" s="2"/>
       <c r="E7" s="2"/>
       <c r="F7" s="2"/>
       <c r="G7" s="10"/>
@@ -5620,13 +4895,653 @@
         <v>5</v>
       </c>
       <c r="B8" s="4" t="s">
+        <v>137</v>
+      </c>
+      <c r="C8" s="4" t="s">
+        <v>138</v>
+      </c>
+      <c r="D8" s="2" t="s">
+        <v>139</v>
+      </c>
+      <c r="E8" s="2"/>
+      <c r="F8" s="2"/>
+      <c r="G8" s="10"/>
+      <c r="H8" s="1"/>
+      <c r="I8" s="1"/>
+      <c r="J8" s="1"/>
+      <c r="K8" s="1"/>
+      <c r="L8" s="1"/>
+    </row>
+    <row r="9" spans="1:12" ht="27" x14ac:dyDescent="0.15">
+      <c r="A9" s="9">
+        <v>6</v>
+      </c>
+      <c r="B9" s="4" t="s">
+        <v>140</v>
+      </c>
+      <c r="C9" s="4" t="s">
+        <v>141</v>
+      </c>
+      <c r="D9" s="2" t="s">
+        <v>142</v>
+      </c>
+      <c r="E9" s="2"/>
+      <c r="F9" s="2"/>
+      <c r="G9" s="10"/>
+      <c r="H9" s="1"/>
+      <c r="I9" s="1"/>
+      <c r="J9" s="1"/>
+      <c r="K9" s="1"/>
+      <c r="L9" s="1"/>
+    </row>
+    <row r="10" spans="1:12" ht="27" x14ac:dyDescent="0.15">
+      <c r="A10" s="9">
+        <v>7</v>
+      </c>
+      <c r="B10" s="4" t="s">
+        <v>143</v>
+      </c>
+      <c r="C10" s="4" t="s">
+        <v>144</v>
+      </c>
+      <c r="D10" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="E10" s="2"/>
+      <c r="F10" s="2"/>
+      <c r="G10" s="10"/>
+      <c r="H10" s="1"/>
+      <c r="I10" s="1"/>
+      <c r="J10" s="1"/>
+      <c r="K10" s="1"/>
+      <c r="L10" s="1"/>
+    </row>
+    <row r="11" spans="1:12" x14ac:dyDescent="0.15">
+      <c r="A11" s="9">
+        <v>8</v>
+      </c>
+      <c r="B11" s="4" t="s">
+        <v>43</v>
+      </c>
+      <c r="C11" s="4" t="s">
+        <v>145</v>
+      </c>
+      <c r="D11" s="4"/>
+      <c r="E11" s="2"/>
+      <c r="F11" s="2"/>
+      <c r="G11" s="10"/>
+      <c r="H11" s="1"/>
+      <c r="I11" s="1"/>
+      <c r="J11" s="1"/>
+      <c r="K11" s="1"/>
+      <c r="L11" s="1"/>
+    </row>
+    <row r="12" spans="1:12" x14ac:dyDescent="0.15">
+      <c r="A12" s="9">
+        <v>9</v>
+      </c>
+      <c r="B12" s="4"/>
+      <c r="C12" s="4"/>
+      <c r="D12" s="4"/>
+      <c r="E12" s="2"/>
+      <c r="F12" s="2"/>
+      <c r="G12" s="10"/>
+      <c r="H12" s="1"/>
+      <c r="I12" s="1"/>
+      <c r="J12" s="1"/>
+      <c r="K12" s="1"/>
+      <c r="L12" s="1"/>
+    </row>
+    <row r="13" spans="1:12" x14ac:dyDescent="0.15">
+      <c r="A13" s="9">
+        <v>10</v>
+      </c>
+      <c r="B13" s="4"/>
+      <c r="C13" s="2"/>
+      <c r="D13" s="2"/>
+      <c r="E13" s="2"/>
+      <c r="F13" s="2"/>
+      <c r="G13" s="10"/>
+      <c r="H13" s="1"/>
+      <c r="I13" s="1"/>
+      <c r="J13" s="1"/>
+      <c r="K13" s="1"/>
+      <c r="L13" s="1"/>
+    </row>
+    <row r="14" spans="1:12" x14ac:dyDescent="0.15">
+      <c r="A14" s="9">
+        <v>11</v>
+      </c>
+      <c r="B14" s="2"/>
+      <c r="C14" s="2"/>
+      <c r="D14" s="2"/>
+      <c r="E14" s="2"/>
+      <c r="F14" s="2"/>
+      <c r="G14" s="10"/>
+      <c r="H14" s="1"/>
+      <c r="I14" s="1"/>
+      <c r="J14" s="1"/>
+      <c r="K14" s="1"/>
+      <c r="L14" s="1"/>
+    </row>
+    <row r="15" spans="1:12" x14ac:dyDescent="0.15">
+      <c r="A15" s="9">
+        <v>12</v>
+      </c>
+      <c r="B15" s="4"/>
+      <c r="C15" s="4"/>
+      <c r="D15" s="4"/>
+      <c r="E15" s="2"/>
+      <c r="F15" s="2"/>
+      <c r="G15" s="10"/>
+      <c r="H15" s="1"/>
+      <c r="I15" s="1"/>
+      <c r="J15" s="1"/>
+      <c r="K15" s="1"/>
+      <c r="L15" s="1"/>
+    </row>
+    <row r="16" spans="1:12" x14ac:dyDescent="0.15">
+      <c r="A16" s="9">
+        <v>13</v>
+      </c>
+      <c r="B16" s="4"/>
+      <c r="C16" s="4"/>
+      <c r="D16" s="4"/>
+      <c r="E16" s="2"/>
+      <c r="F16" s="2"/>
+      <c r="G16" s="10"/>
+      <c r="H16" s="1"/>
+      <c r="I16" s="1"/>
+      <c r="J16" s="1"/>
+      <c r="K16" s="1"/>
+      <c r="L16" s="1"/>
+    </row>
+    <row r="17" spans="1:12" x14ac:dyDescent="0.15">
+      <c r="A17" s="9">
+        <v>14</v>
+      </c>
+      <c r="B17" s="4"/>
+      <c r="C17" s="4"/>
+      <c r="D17" s="4"/>
+      <c r="E17" s="2"/>
+      <c r="F17" s="2"/>
+      <c r="G17" s="10"/>
+      <c r="H17" s="1"/>
+      <c r="I17" s="1"/>
+      <c r="J17" s="1"/>
+      <c r="K17" s="1"/>
+      <c r="L17" s="1"/>
+    </row>
+    <row r="18" spans="1:12" x14ac:dyDescent="0.15">
+      <c r="A18" s="9">
+        <v>15</v>
+      </c>
+      <c r="B18" s="4"/>
+      <c r="C18" s="4"/>
+      <c r="D18" s="4"/>
+      <c r="E18" s="2"/>
+      <c r="F18" s="2"/>
+      <c r="G18" s="10"/>
+      <c r="H18" s="1"/>
+      <c r="I18" s="1"/>
+      <c r="J18" s="1"/>
+      <c r="K18" s="1"/>
+      <c r="L18" s="1"/>
+    </row>
+    <row r="19" spans="1:12" x14ac:dyDescent="0.15">
+      <c r="A19" s="9">
+        <v>16</v>
+      </c>
+      <c r="B19" s="6"/>
+      <c r="C19" s="6"/>
+      <c r="D19" s="6"/>
+      <c r="E19" s="2"/>
+      <c r="F19" s="2"/>
+      <c r="G19" s="10"/>
+      <c r="H19" s="1"/>
+      <c r="I19" s="1"/>
+      <c r="J19" s="1"/>
+      <c r="K19" s="1"/>
+      <c r="L19" s="1"/>
+    </row>
+    <row r="20" spans="1:12" x14ac:dyDescent="0.15">
+      <c r="A20" s="9">
+        <v>17</v>
+      </c>
+      <c r="B20" s="4"/>
+      <c r="C20" s="4"/>
+      <c r="D20" s="6"/>
+      <c r="E20" s="2"/>
+      <c r="F20" s="2"/>
+      <c r="G20" s="10"/>
+      <c r="H20" s="1"/>
+      <c r="I20" s="1"/>
+      <c r="J20" s="1"/>
+      <c r="K20" s="1"/>
+      <c r="L20" s="1"/>
+    </row>
+    <row r="21" spans="1:12" x14ac:dyDescent="0.15">
+      <c r="A21" s="9">
+        <v>18</v>
+      </c>
+      <c r="B21" s="4"/>
+      <c r="C21" s="4"/>
+      <c r="D21" s="6"/>
+      <c r="E21" s="2"/>
+      <c r="F21" s="2"/>
+      <c r="G21" s="10"/>
+      <c r="H21" s="1"/>
+      <c r="I21" s="1"/>
+      <c r="J21" s="1"/>
+      <c r="K21" s="1"/>
+      <c r="L21" s="1"/>
+    </row>
+    <row r="22" spans="1:12" x14ac:dyDescent="0.15">
+      <c r="A22" s="9">
+        <v>19</v>
+      </c>
+      <c r="B22" s="4"/>
+      <c r="C22" s="4"/>
+      <c r="D22" s="6"/>
+      <c r="E22" s="2"/>
+      <c r="F22" s="2"/>
+      <c r="G22" s="10"/>
+      <c r="H22" s="1"/>
+      <c r="I22" s="1"/>
+      <c r="J22" s="1"/>
+      <c r="K22" s="1"/>
+      <c r="L22" s="1"/>
+    </row>
+    <row r="23" spans="1:12" x14ac:dyDescent="0.15">
+      <c r="A23" s="11">
+        <v>20</v>
+      </c>
+      <c r="B23" s="6"/>
+      <c r="C23" s="6"/>
+      <c r="D23" s="6"/>
+      <c r="E23" s="7"/>
+      <c r="F23" s="7"/>
+      <c r="G23" s="12"/>
+      <c r="H23" s="1"/>
+      <c r="I23" s="1"/>
+      <c r="J23" s="1"/>
+      <c r="K23" s="1"/>
+      <c r="L23" s="1"/>
+    </row>
+    <row r="24" spans="1:12" s="1" customFormat="1" x14ac:dyDescent="0.15">
+      <c r="A24" s="2">
+        <v>21</v>
+      </c>
+      <c r="B24" s="4"/>
+      <c r="C24" s="4"/>
+      <c r="D24" s="4"/>
+      <c r="E24" s="2"/>
+      <c r="F24" s="2"/>
+      <c r="G24" s="10"/>
+    </row>
+    <row r="25" spans="1:12" x14ac:dyDescent="0.15">
+      <c r="A25" s="13">
+        <v>22</v>
+      </c>
+      <c r="B25" s="14"/>
+      <c r="C25" s="14"/>
+      <c r="D25" s="15"/>
+      <c r="E25" s="15"/>
+      <c r="F25" s="15"/>
+      <c r="G25" s="16"/>
+      <c r="H25" s="1"/>
+      <c r="I25" s="1"/>
+      <c r="J25" s="1"/>
+      <c r="K25" s="1"/>
+      <c r="L25" s="1"/>
+    </row>
+    <row r="26" spans="1:12" x14ac:dyDescent="0.15">
+      <c r="A26" s="9">
+        <v>23</v>
+      </c>
+      <c r="B26" s="8"/>
+      <c r="C26" s="8"/>
+      <c r="D26" s="4"/>
+      <c r="E26" s="2"/>
+      <c r="F26" s="2"/>
+      <c r="G26" s="10"/>
+      <c r="H26" s="1"/>
+      <c r="I26" s="1"/>
+      <c r="J26" s="1"/>
+      <c r="K26" s="1"/>
+      <c r="L26" s="1"/>
+    </row>
+    <row r="27" spans="1:12" x14ac:dyDescent="0.15">
+      <c r="A27" s="9">
+        <v>24</v>
+      </c>
+      <c r="B27" s="8"/>
+      <c r="C27" s="8"/>
+      <c r="D27" s="4"/>
+      <c r="E27" s="2"/>
+      <c r="F27" s="2"/>
+      <c r="G27" s="10"/>
+      <c r="H27" s="1"/>
+      <c r="I27" s="1"/>
+      <c r="J27" s="1"/>
+      <c r="K27" s="1"/>
+      <c r="L27" s="1"/>
+    </row>
+    <row r="28" spans="1:12" x14ac:dyDescent="0.15">
+      <c r="A28" s="9">
+        <v>25</v>
+      </c>
+      <c r="B28" s="4"/>
+      <c r="C28" s="8"/>
+      <c r="D28" s="4"/>
+      <c r="E28" s="2"/>
+      <c r="F28" s="2"/>
+      <c r="G28" s="10"/>
+    </row>
+    <row r="29" spans="1:12" x14ac:dyDescent="0.15">
+      <c r="A29" s="9">
+        <v>26</v>
+      </c>
+      <c r="B29" s="4"/>
+      <c r="C29" s="8"/>
+      <c r="D29" s="4"/>
+      <c r="E29" s="2"/>
+      <c r="F29" s="2"/>
+      <c r="G29" s="10"/>
+    </row>
+    <row r="30" spans="1:12" x14ac:dyDescent="0.15">
+      <c r="A30" s="9">
+        <v>27</v>
+      </c>
+      <c r="B30" s="4"/>
+      <c r="C30" s="8"/>
+      <c r="D30" s="4"/>
+      <c r="E30" s="2"/>
+      <c r="F30" s="2"/>
+      <c r="G30" s="10"/>
+    </row>
+    <row r="31" spans="1:12" x14ac:dyDescent="0.15">
+      <c r="A31" s="9">
+        <v>28</v>
+      </c>
+      <c r="B31" s="4"/>
+      <c r="C31" s="8"/>
+      <c r="D31" s="4"/>
+      <c r="E31" s="2"/>
+      <c r="F31" s="2"/>
+      <c r="G31" s="10"/>
+    </row>
+    <row r="32" spans="1:12" x14ac:dyDescent="0.15">
+      <c r="A32" s="9">
+        <v>29</v>
+      </c>
+      <c r="B32" s="4"/>
+      <c r="C32" s="8"/>
+      <c r="D32" s="4"/>
+      <c r="E32" s="2"/>
+      <c r="F32" s="2"/>
+      <c r="G32" s="10"/>
+    </row>
+    <row r="33" spans="1:7" x14ac:dyDescent="0.15">
+      <c r="A33" s="9">
+        <v>30</v>
+      </c>
+      <c r="B33" s="4"/>
+      <c r="C33" s="8"/>
+      <c r="D33" s="4"/>
+      <c r="E33" s="2"/>
+      <c r="F33" s="2"/>
+      <c r="G33" s="10"/>
+    </row>
+    <row r="34" spans="1:7" x14ac:dyDescent="0.15">
+      <c r="A34" s="9">
+        <v>31</v>
+      </c>
+      <c r="B34" s="4"/>
+      <c r="C34" s="8"/>
+      <c r="D34" s="4"/>
+      <c r="E34" s="2"/>
+      <c r="F34" s="2"/>
+      <c r="G34" s="10"/>
+    </row>
+    <row r="35" spans="1:7" x14ac:dyDescent="0.15">
+      <c r="A35" s="9">
+        <v>32</v>
+      </c>
+      <c r="B35" s="4"/>
+      <c r="C35" s="8"/>
+      <c r="D35" s="4"/>
+      <c r="E35" s="2"/>
+      <c r="F35" s="2"/>
+      <c r="G35" s="10"/>
+    </row>
+    <row r="36" spans="1:7" x14ac:dyDescent="0.15">
+      <c r="A36" s="9">
+        <v>33</v>
+      </c>
+      <c r="B36" s="4"/>
+      <c r="C36" s="8"/>
+      <c r="D36" s="4"/>
+      <c r="E36" s="2"/>
+      <c r="F36" s="2"/>
+      <c r="G36" s="10"/>
+    </row>
+    <row r="37" spans="1:7" x14ac:dyDescent="0.15">
+      <c r="A37" s="9">
+        <v>34</v>
+      </c>
+      <c r="B37" s="4"/>
+      <c r="C37" s="8"/>
+      <c r="D37" s="4"/>
+      <c r="E37" s="2"/>
+      <c r="F37" s="2"/>
+      <c r="G37" s="10"/>
+    </row>
+    <row r="38" spans="1:7" x14ac:dyDescent="0.15">
+      <c r="A38" s="9">
+        <v>35</v>
+      </c>
+      <c r="B38" s="4"/>
+      <c r="C38" s="8"/>
+      <c r="D38" s="4"/>
+      <c r="E38" s="2"/>
+      <c r="F38" s="2"/>
+      <c r="G38" s="10"/>
+    </row>
+    <row r="39" spans="1:7" x14ac:dyDescent="0.15">
+      <c r="A39" s="9">
+        <v>36</v>
+      </c>
+      <c r="B39" s="4"/>
+      <c r="C39" s="8"/>
+      <c r="D39" s="4"/>
+      <c r="E39" s="2"/>
+      <c r="F39" s="2"/>
+      <c r="G39" s="10"/>
+    </row>
+    <row r="40" spans="1:7" x14ac:dyDescent="0.15">
+      <c r="A40" s="9">
+        <v>37</v>
+      </c>
+      <c r="B40" s="4"/>
+      <c r="C40" s="8"/>
+      <c r="D40" s="4"/>
+      <c r="E40" s="2"/>
+      <c r="F40" s="2"/>
+      <c r="G40" s="10"/>
+    </row>
+    <row r="41" spans="1:7" x14ac:dyDescent="0.15">
+      <c r="A41" s="9">
+        <v>38</v>
+      </c>
+      <c r="B41" s="4"/>
+      <c r="C41" s="4"/>
+      <c r="D41" s="4"/>
+      <c r="E41" s="2"/>
+      <c r="F41" s="2"/>
+      <c r="G41" s="10"/>
+    </row>
+    <row r="42" spans="1:7" x14ac:dyDescent="0.15">
+      <c r="A42" s="9">
+        <v>39</v>
+      </c>
+      <c r="B42" s="4"/>
+      <c r="C42" s="4"/>
+      <c r="D42" s="4"/>
+      <c r="E42" s="2"/>
+      <c r="F42" s="2"/>
+      <c r="G42" s="10"/>
+    </row>
+    <row r="43" spans="1:7" x14ac:dyDescent="0.15">
+      <c r="A43" s="9">
+        <v>40</v>
+      </c>
+      <c r="B43" s="4"/>
+      <c r="C43" s="4"/>
+      <c r="D43" s="4"/>
+      <c r="E43" s="2"/>
+      <c r="F43" s="2"/>
+      <c r="G43" s="10"/>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="1"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="360" verticalDpi="360" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:L43"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B8" sqref="B8:D8"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
+  <cols>
+    <col min="1" max="1" width="3.25" customWidth="1"/>
+    <col min="2" max="2" width="17.375" customWidth="1"/>
+    <col min="3" max="3" width="57.625" customWidth="1"/>
+    <col min="4" max="4" width="45.125" customWidth="1"/>
+    <col min="5" max="5" width="12.625" customWidth="1"/>
+    <col min="6" max="6" width="11.625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:12" ht="17.25" x14ac:dyDescent="0.15">
+      <c r="A1" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="C1" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="3" spans="1:12" x14ac:dyDescent="0.15">
+      <c r="A3" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="D3" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="E3" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="F3" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="G3" s="5" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="4" spans="1:12" x14ac:dyDescent="0.15">
+      <c r="A4" s="9">
+        <v>1</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="C4" s="4" t="s">
+        <v>45</v>
+      </c>
+      <c r="D4" s="2" t="s">
+        <v>146</v>
+      </c>
+      <c r="E4" s="2"/>
+      <c r="F4" s="2"/>
+      <c r="G4" s="10"/>
+    </row>
+    <row r="5" spans="1:12" ht="27" x14ac:dyDescent="0.15">
+      <c r="A5" s="9">
+        <v>2</v>
+      </c>
+      <c r="B5" s="4" t="s">
+        <v>46</v>
+      </c>
+      <c r="C5" s="4" t="s">
+        <v>47</v>
+      </c>
+      <c r="D5" s="19"/>
+      <c r="E5" s="2"/>
+      <c r="F5" s="2"/>
+      <c r="G5" s="10"/>
+    </row>
+    <row r="6" spans="1:12" x14ac:dyDescent="0.15">
+      <c r="A6" s="9">
+        <v>3</v>
+      </c>
+      <c r="B6" s="4" t="s">
+        <v>48</v>
+      </c>
+      <c r="C6" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="D6" s="2" t="s">
+        <v>147</v>
+      </c>
+      <c r="E6" s="2"/>
+      <c r="F6" s="2"/>
+      <c r="G6" s="10"/>
+    </row>
+    <row r="7" spans="1:12" ht="27" x14ac:dyDescent="0.15">
+      <c r="A7" s="9">
+        <v>4</v>
+      </c>
+      <c r="B7" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="C7" s="4" t="s">
+        <v>148</v>
+      </c>
+      <c r="D7" s="2" t="s">
+        <v>149</v>
+      </c>
+      <c r="E7" s="2"/>
+      <c r="F7" s="2"/>
+      <c r="G7" s="10"/>
+      <c r="H7" s="1"/>
+      <c r="I7" s="1"/>
+      <c r="J7" s="1"/>
+      <c r="K7" s="1"/>
+      <c r="L7" s="1"/>
+    </row>
+    <row r="8" spans="1:12" ht="27" x14ac:dyDescent="0.15">
+      <c r="A8" s="9">
+        <v>5</v>
+      </c>
+      <c r="B8" s="4" t="s">
         <v>9</v>
       </c>
       <c r="C8" s="4" t="s">
         <v>10</v>
       </c>
       <c r="D8" s="17" t="s">
-        <v>164</v>
+        <v>166</v>
       </c>
       <c r="E8" s="2"/>
       <c r="F8" s="2"/>
@@ -6301,10 +6216,10 @@
         <v>8</v>
       </c>
       <c r="B11" s="4" t="s">
-        <v>162</v>
+        <v>164</v>
       </c>
       <c r="C11" s="4" t="s">
-        <v>168</v>
+        <v>170</v>
       </c>
       <c r="D11" s="4"/>
       <c r="E11" s="2"/>
@@ -6755,8 +6670,8 @@
   <sheetPr codeName="Sheet8"/>
   <dimension ref="A1:L44"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D7" sqref="D7"/>
+    <sheetView topLeftCell="A2" workbookViewId="0">
+      <selection activeCell="A7" sqref="A7:D7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
@@ -6823,7 +6738,7 @@
         <v>62</v>
       </c>
       <c r="C5" s="4" t="s">
-        <v>166</v>
+        <v>168</v>
       </c>
       <c r="D5" s="4"/>
       <c r="E5" s="2"/>
@@ -6835,14 +6750,12 @@
         <v>3</v>
       </c>
       <c r="B6" s="4" t="s">
-        <v>152</v>
+        <v>154</v>
       </c>
       <c r="C6" s="18" t="s">
-        <v>153</v>
-      </c>
-      <c r="D6" s="22" t="s">
-        <v>176</v>
-      </c>
+        <v>155</v>
+      </c>
+      <c r="D6" s="22"/>
       <c r="E6" s="2"/>
       <c r="F6" s="2"/>
       <c r="G6" s="10"/>
@@ -6852,14 +6765,12 @@
         <v>4</v>
       </c>
       <c r="B7" s="4" t="s">
-        <v>167</v>
+        <v>169</v>
       </c>
       <c r="C7" s="18" t="s">
-        <v>169</v>
-      </c>
-      <c r="D7" s="21" t="s">
-        <v>177</v>
-      </c>
+        <v>171</v>
+      </c>
+      <c r="D7" s="22"/>
       <c r="E7" s="2"/>
       <c r="F7" s="2"/>
       <c r="G7" s="10"/>
@@ -6869,10 +6780,10 @@
         <v>5</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>154</v>
+        <v>156</v>
       </c>
       <c r="C8" s="18" t="s">
-        <v>155</v>
+        <v>157</v>
       </c>
       <c r="D8" s="2"/>
       <c r="E8" s="2"/>
@@ -6889,10 +6800,10 @@
         <v>6</v>
       </c>
       <c r="B9" s="4" t="s">
-        <v>156</v>
+        <v>158</v>
       </c>
       <c r="C9" s="18" t="s">
-        <v>157</v>
+        <v>159</v>
       </c>
       <c r="D9" s="2"/>
       <c r="E9" s="2"/>
@@ -6909,10 +6820,10 @@
         <v>7</v>
       </c>
       <c r="B10" s="4" t="s">
-        <v>158</v>
+        <v>160</v>
       </c>
       <c r="C10" s="18" t="s">
-        <v>159</v>
+        <v>161</v>
       </c>
       <c r="D10" s="2"/>
       <c r="E10" s="2"/>
@@ -6969,10 +6880,10 @@
         <v>10</v>
       </c>
       <c r="B13" s="4" t="s">
-        <v>160</v>
+        <v>162</v>
       </c>
       <c r="C13" s="4" t="s">
-        <v>161</v>
+        <v>163</v>
       </c>
       <c r="D13" s="4"/>
       <c r="E13" s="2"/>
@@ -6989,10 +6900,10 @@
         <v>11</v>
       </c>
       <c r="B14" s="4" t="s">
-        <v>162</v>
+        <v>164</v>
       </c>
       <c r="C14" s="4" t="s">
-        <v>163</v>
+        <v>165</v>
       </c>
       <c r="D14" s="4"/>
       <c r="E14" s="2"/>
@@ -7412,7 +7323,7 @@
   <dimension ref="A1:L44"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D7" sqref="D7"/>
+      <selection activeCell="B7" sqref="B7:D7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
@@ -7476,7 +7387,7 @@
         <v>62</v>
       </c>
       <c r="C5" s="4" t="s">
-        <v>151</v>
+        <v>153</v>
       </c>
       <c r="D5" s="4"/>
       <c r="E5" s="2"/>
@@ -7488,14 +7399,12 @@
         <v>3</v>
       </c>
       <c r="B6" s="4" t="s">
-        <v>152</v>
+        <v>154</v>
       </c>
       <c r="C6" s="18" t="s">
-        <v>153</v>
-      </c>
-      <c r="D6" s="21" t="s">
-        <v>178</v>
-      </c>
+        <v>155</v>
+      </c>
+      <c r="D6" s="2"/>
       <c r="E6" s="2"/>
       <c r="F6" s="2"/>
       <c r="G6" s="10"/>
@@ -7505,14 +7414,12 @@
         <v>4</v>
       </c>
       <c r="B7" s="4" t="s">
-        <v>167</v>
+        <v>169</v>
       </c>
       <c r="C7" s="18" t="s">
-        <v>169</v>
-      </c>
-      <c r="D7" s="21" t="s">
-        <v>179</v>
-      </c>
+        <v>171</v>
+      </c>
+      <c r="D7" s="22"/>
       <c r="E7" s="2"/>
       <c r="F7" s="2"/>
       <c r="G7" s="10"/>
@@ -7522,10 +7429,10 @@
         <v>5</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>154</v>
+        <v>156</v>
       </c>
       <c r="C8" s="18" t="s">
-        <v>155</v>
+        <v>157</v>
       </c>
       <c r="D8" s="2"/>
       <c r="E8" s="2"/>
@@ -7542,10 +7449,10 @@
         <v>6</v>
       </c>
       <c r="B9" s="4" t="s">
-        <v>156</v>
+        <v>158</v>
       </c>
       <c r="C9" s="18" t="s">
-        <v>157</v>
+        <v>159</v>
       </c>
       <c r="D9" s="2"/>
       <c r="E9" s="2"/>
@@ -7562,10 +7469,10 @@
         <v>7</v>
       </c>
       <c r="B10" s="4" t="s">
-        <v>158</v>
+        <v>160</v>
       </c>
       <c r="C10" s="18" t="s">
-        <v>159</v>
+        <v>161</v>
       </c>
       <c r="D10" s="2"/>
       <c r="E10" s="2"/>
@@ -7622,10 +7529,10 @@
         <v>10</v>
       </c>
       <c r="B13" s="4" t="s">
-        <v>160</v>
+        <v>162</v>
       </c>
       <c r="C13" s="4" t="s">
-        <v>161</v>
+        <v>163</v>
       </c>
       <c r="D13" s="4"/>
       <c r="E13" s="2"/>
@@ -7642,10 +7549,10 @@
         <v>11</v>
       </c>
       <c r="B14" s="4" t="s">
-        <v>162</v>
+        <v>164</v>
       </c>
       <c r="C14" s="4" t="s">
-        <v>163</v>
+        <v>165</v>
       </c>
       <c r="D14" s="4"/>
       <c r="E14" s="2"/>
@@ -8064,8 +7971,8 @@
   <sheetPr codeName="Sheet10"/>
   <dimension ref="A1:L44"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D7" sqref="D7"/>
+    <sheetView topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="B14" sqref="B14:C14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
@@ -8129,7 +8036,7 @@
         <v>62</v>
       </c>
       <c r="C5" s="4" t="s">
-        <v>151</v>
+        <v>153</v>
       </c>
       <c r="D5" s="4"/>
       <c r="E5" s="2"/>
@@ -8141,14 +8048,12 @@
         <v>3</v>
       </c>
       <c r="B6" s="4" t="s">
-        <v>152</v>
+        <v>154</v>
       </c>
       <c r="C6" s="18" t="s">
-        <v>153</v>
-      </c>
-      <c r="D6" s="21" t="s">
-        <v>180</v>
-      </c>
+        <v>155</v>
+      </c>
+      <c r="D6" s="2"/>
       <c r="E6" s="2"/>
       <c r="F6" s="2"/>
       <c r="G6" s="10"/>
@@ -8158,14 +8063,12 @@
         <v>4</v>
       </c>
       <c r="B7" s="4" t="s">
-        <v>167</v>
+        <v>169</v>
       </c>
       <c r="C7" s="18" t="s">
-        <v>169</v>
-      </c>
-      <c r="D7" s="21" t="s">
-        <v>181</v>
-      </c>
+        <v>171</v>
+      </c>
+      <c r="D7" s="22"/>
       <c r="E7" s="2"/>
       <c r="F7" s="2"/>
       <c r="G7" s="10"/>
@@ -8175,10 +8078,10 @@
         <v>5</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>154</v>
+        <v>156</v>
       </c>
       <c r="C8" s="18" t="s">
-        <v>155</v>
+        <v>157</v>
       </c>
       <c r="D8" s="2"/>
       <c r="E8" s="2"/>
@@ -8195,10 +8098,10 @@
         <v>6</v>
       </c>
       <c r="B9" s="4" t="s">
-        <v>156</v>
+        <v>158</v>
       </c>
       <c r="C9" s="18" t="s">
-        <v>157</v>
+        <v>159</v>
       </c>
       <c r="D9" s="2"/>
       <c r="E9" s="2"/>
@@ -8215,10 +8118,10 @@
         <v>7</v>
       </c>
       <c r="B10" s="4" t="s">
-        <v>158</v>
+        <v>160</v>
       </c>
       <c r="C10" s="18" t="s">
-        <v>159</v>
+        <v>161</v>
       </c>
       <c r="D10" s="2"/>
       <c r="E10" s="2"/>
@@ -8275,10 +8178,10 @@
         <v>10</v>
       </c>
       <c r="B13" s="4" t="s">
-        <v>160</v>
+        <v>162</v>
       </c>
       <c r="C13" s="4" t="s">
-        <v>161</v>
+        <v>163</v>
       </c>
       <c r="D13" s="4"/>
       <c r="E13" s="2"/>
@@ -8295,10 +8198,10 @@
         <v>11</v>
       </c>
       <c r="B14" s="4" t="s">
-        <v>162</v>
+        <v>164</v>
       </c>
       <c r="C14" s="4" t="s">
-        <v>163</v>
+        <v>165</v>
       </c>
       <c r="D14" s="4"/>
       <c r="E14" s="2"/>
@@ -8718,7 +8621,7 @@
   <dimension ref="A1:L43"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C5" sqref="C5"/>
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
@@ -8736,7 +8639,7 @@
         <v>7</v>
       </c>
       <c r="C1" t="s">
-        <v>170</v>
+        <v>172</v>
       </c>
     </row>
     <row r="3" spans="1:12" x14ac:dyDescent="0.15">
@@ -8796,8 +8699,12 @@
       <c r="A6" s="9">
         <v>3</v>
       </c>
-      <c r="B6" s="4"/>
-      <c r="C6" s="4"/>
+      <c r="B6" s="4" t="s">
+        <v>164</v>
+      </c>
+      <c r="C6" s="4" t="s">
+        <v>165</v>
+      </c>
       <c r="D6" s="2"/>
       <c r="E6" s="2"/>
       <c r="F6" s="2"/>
@@ -9322,8 +9229,8 @@
   <sheetPr codeName="Sheet6"/>
   <dimension ref="A1:L43"/>
   <sheetViews>
-    <sheetView topLeftCell="A19" workbookViewId="0">
-      <selection activeCell="C13" sqref="C13"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
@@ -9486,7 +9393,7 @@
         <v>67</v>
       </c>
       <c r="C10" s="4" t="s">
-        <v>148</v>
+        <v>150</v>
       </c>
       <c r="D10" s="2"/>
       <c r="E10" s="2"/>
@@ -9503,10 +9410,10 @@
         <v>8</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>149</v>
+        <v>151</v>
       </c>
       <c r="C11" s="4" t="s">
-        <v>150</v>
+        <v>152</v>
       </c>
       <c r="D11" s="2"/>
       <c r="E11" s="2"/>

</xml_diff>